<commit_message>
avance en documento de análisis
</commit_message>
<xml_diff>
--- a/Docs/Gráficas máquina 1.xlsx
+++ b/Docs/Gráficas máquina 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Reto 4\Reto4-G10\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125EC4A7-6C2E-44EE-B48A-C734BF022739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5C4955-7CEE-44E2-A3A7-5A194FB1E135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{674F7855-6ABB-4172-9BD7-8DDF58622BAF}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Requerimiento</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Conocer el impacto que tendría el fallo de un determinado landing point</t>
+  </si>
+  <si>
+    <t>Carga de datos</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -137,19 +140,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -168,6 +178,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,7 +294,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos de rendimiento'!$B$2</c:f>
+              <c:f>'Datos de rendimiento'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -353,22 +375,25 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Datos de rendimiento'!$A$3:$A$8</c:f>
+              <c:f>'Datos de rendimiento'!$B$3:$B$8</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Carga de datos</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Encontrar cantidad de clusteres dentro de la red de cables submarinos</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Encontrar landing points que sirven como punto de interconexión a más cables</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Encontrar la ruta mínima para enviar información entre dos países</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Identificar la infraestructura crítica para garantizar el mantenimiento preventivo</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Conocer el impacto que tendría el fallo de un determinado landing point</c:v>
                 </c:pt>
               </c:strCache>
@@ -376,10 +401,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos de rendimiento'!$B$3:$B$8</c:f>
+              <c:f>'Datos de rendimiento'!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>830.45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6242.1639999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1989.357</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -595,7 +629,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -837,7 +871,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Datos de rendimiento'!$B$13</c:f>
+              <c:f>'Datos de rendimiento'!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -918,22 +952,25 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Datos de rendimiento'!$A$14:$A$19</c:f>
+              <c:f>'Datos de rendimiento'!$B$14:$B$19</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>Carga de datos</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>Encontrar cantidad de clusteres dentro de la red de cables submarinos</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>Encontrar landing points que sirven como punto de interconexión a más cables</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>Encontrar la ruta mínima para enviar información entre dos países</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Identificar la infraestructura crítica para garantizar el mantenimiento preventivo</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>Conocer el impacto que tendría el fallo de un determinado landing point</c:v>
                 </c:pt>
               </c:strCache>
@@ -941,10 +978,19 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Datos de rendimiento'!$B$14:$B$19</c:f>
+              <c:f>'Datos de rendimiento'!$C$14:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.000</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1046.4380000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117.63200000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.044</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -975,61 +1021,6 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="es-CO" b="1"/>
-                  <a:t>Requerimiento</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-CO"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1078,7 +1069,7 @@
         <c:axId val="92093976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="20"/>
+          <c:max val="1050"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2774,117 +2765,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2B8949-CC7B-4468-84E4-E8B7F9651F12}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="4"/>
-      <c r="B1" s="3"/>
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B1" s="12"/>
+      <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
+        <v>0</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="17">
+        <v>830.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="C4" s="7">
+        <v>6242.1639999999998</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>2</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="C5" s="7"/>
     </row>
-    <row r="5" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10"/>
+      <c r="C6" s="8">
+        <v>1989.357</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10"/>
+      <c r="C7" s="8"/>
     </row>
-    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="C8" s="8"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="10"/>
+    <row r="9" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
+    <row r="10" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
+    <row r="11" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
+    <row r="12" spans="1:3" s="9" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="C12" s="11"/>
     </row>
-    <row r="12" spans="1:2" s="11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="13"/>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="B13" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
         <v>0</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1046.4380000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
         <v>1</v>
       </c>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>117.63200000000001</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
+        <v>2</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
         <v>3</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>21.044</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
         <v>4</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="1"/>
     </row>
-    <row r="16" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="7" t="s">
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
         <v>5</v>
       </c>
-      <c r="B16" s="1"/>
-    </row>
-    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7" t="s">
+      <c r="B19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
-      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cambios en documento de observaciones y gráficas
</commit_message>
<xml_diff>
--- a/Docs/Gráficas máquina 1.xlsx
+++ b/Docs/Gráficas máquina 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Reto 4\Reto4-G10\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5C4955-7CEE-44E2-A3A7-5A194FB1E135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D4C14E-5AD7-4AFE-B166-E952C6B1153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{674F7855-6ABB-4172-9BD7-8DDF58622BAF}"/>
   </bookViews>
@@ -406,13 +406,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>830.45</c:v>
+                  <c:v>510.608</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6242.1639999999998</c:v>
+                  <c:v>4042.2269999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1989.357</c:v>
+                  <c:v>1221.357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -983,7 +983,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1046.4380000000001</c:v>
+                  <c:v>1046.019</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>117.63200000000001</c:v>
@@ -2768,7 +2768,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2798,7 +2798,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="17">
-        <v>830.45</v>
+        <v>510.608</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -2809,7 +2809,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="7">
-        <v>6242.1639999999998</v>
+        <v>4042.2269999999999</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -2829,7 +2829,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8">
-        <v>1989.357</v>
+        <v>1221.357</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -2878,7 +2878,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="1">
-        <v>1046.4380000000001</v>
+        <v>1046.019</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>